<commit_message>
table sst dc results
</commit_message>
<xml_diff>
--- a/expresults.xlsx
+++ b/expresults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ansonthai/Downloads/summer-research-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63FC5308-4AF9-FC4E-8C09-D9AA80AA25ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1BF305-D918-8248-91B1-F6702DDD6CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19600" yWindow="4460" windowWidth="33600" windowHeight="21000" activeTab="3" xr2:uid="{545D3D87-BFDF-DF4F-A4B6-49EF553C2706}"/>
+    <workbookView xWindow="17600" yWindow="5980" windowWidth="33600" windowHeight="21000" activeTab="3" xr2:uid="{545D3D87-BFDF-DF4F-A4B6-49EF553C2706}"/>
   </bookViews>
   <sheets>
     <sheet name="Indexing" sheetId="1" r:id="rId1"/>
@@ -610,7 +610,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -622,16 +632,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1236,7 +1236,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Query Evaluation'!$A$25</c:f>
+              <c:f>'Query Evaluation V2'!$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1271,7 +1271,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Query Evaluation'!$B$24:$E$24</c:f>
+              <c:f>'Query Evaluation V2'!$B$23:$E$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1292,7 +1292,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Query Evaluation'!$B$25:$E$25</c:f>
+              <c:f>'Query Evaluation V2'!$B$24:$E$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1314,7 +1314,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5439-B147-8D84-16DB8CBF29E9}"/>
+              <c16:uniqueId val="{00000000-484E-C84E-9434-2222F57A6AF7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1323,7 +1323,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Query Evaluation'!$A$26</c:f>
+              <c:f>'Query Evaluation V2'!$A$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1358,7 +1358,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Query Evaluation'!$B$24:$E$24</c:f>
+              <c:f>'Query Evaluation V2'!$B$23:$E$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1379,7 +1379,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Query Evaluation'!$B$26:$E$26</c:f>
+              <c:f>'Query Evaluation V2'!$B$25:$E$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1401,7 +1401,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-5439-B147-8D84-16DB8CBF29E9}"/>
+              <c16:uniqueId val="{00000001-484E-C84E-9434-2222F57A6AF7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1410,7 +1410,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Query Evaluation'!$A$27</c:f>
+              <c:f>'Query Evaluation V2'!$A$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1445,7 +1445,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Query Evaluation'!$B$24:$E$24</c:f>
+              <c:f>'Query Evaluation V2'!$B$23:$E$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1466,7 +1466,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Query Evaluation'!$B$27:$E$27</c:f>
+              <c:f>'Query Evaluation V2'!$B$26:$E$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1488,7 +1488,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-5439-B147-8D84-16DB8CBF29E9}"/>
+              <c16:uniqueId val="{00000002-484E-C84E-9434-2222F57A6AF7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1496,7 +1496,15 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>table-sst</c:v>
+            <c:strRef>
+              <c:f>'Query Evaluation V2'!$A$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>table-sst</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -1567,7 +1575,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-5439-B147-8D84-16DB8CBF29E9}"/>
+              <c16:uniqueId val="{00000003-484E-C84E-9434-2222F57A6AF7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1637,16 +1645,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1288.8258796236628</c:v>
+                  <c:v>2483.8549428713363</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>393.12193856290344</c:v>
+                  <c:v>901.85963456647607</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>476.96497646177846</c:v>
+                  <c:v>758.48363950789587</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>561.30897252392583</c:v>
+                  <c:v>641.543811026855</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1654,7 +1662,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-5439-B147-8D84-16DB8CBF29E9}"/>
+              <c16:uniqueId val="{00000005-484E-C84E-9434-2222F57A6AF7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1666,11 +1674,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="70292447"/>
-        <c:axId val="124767887"/>
+        <c:axId val="1615604336"/>
+        <c:axId val="1615284304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="70292447"/>
+        <c:axId val="1615604336"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1699,7 +1707,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1713,11 +1721,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB" sz="1500"/>
-                  <a:t>No. of</a:t>
+                  <a:t>Number</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" sz="1500" baseline="0"/>
-                  <a:t> Requests</a:t>
+                  <a:t> of Requests</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-GB" sz="1500"/>
               </a:p>
@@ -1736,7 +1744,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1752,7 +1760,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1789,12 +1797,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="124767887"/>
+        <c:crossAx val="1615284304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="124767887"/>
+        <c:axId val="1615284304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1906,7 +1914,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70292447"/>
+        <c:crossAx val="1615604336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2018,7 +2026,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Query Evaluation'!$A$31</c:f>
+              <c:f>'Query Evaluation V2'!$A$32</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2053,7 +2061,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Query Evaluation'!$B$30:$E$30</c:f>
+              <c:f>'Query Evaluation V2'!$B$31:$E$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2074,7 +2082,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Query Evaluation'!$B$31:$E$31</c:f>
+              <c:f>'Query Evaluation V2'!$B$32:$E$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2096,7 +2104,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-37D7-0548-889D-8F6CD5AE1EB9}"/>
+              <c16:uniqueId val="{00000000-3338-F04B-8E23-C05DF3260C71}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2105,7 +2113,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Query Evaluation'!$A$32</c:f>
+              <c:f>'Query Evaluation V2'!$A$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2140,7 +2148,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Query Evaluation'!$B$30:$E$30</c:f>
+              <c:f>'Query Evaluation V2'!$B$31:$E$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2161,7 +2169,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Query Evaluation'!$B$32:$E$32</c:f>
+              <c:f>'Query Evaluation V2'!$B$33:$E$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2183,7 +2191,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-37D7-0548-889D-8F6CD5AE1EB9}"/>
+              <c16:uniqueId val="{00000001-3338-F04B-8E23-C05DF3260C71}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2192,7 +2200,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Query Evaluation'!$A$33</c:f>
+              <c:f>'Query Evaluation V2'!$A$34</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2227,7 +2235,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Query Evaluation'!$B$30:$E$30</c:f>
+              <c:f>'Query Evaluation V2'!$B$31:$E$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2248,7 +2256,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Query Evaluation'!$B$33:$E$33</c:f>
+              <c:f>'Query Evaluation V2'!$B$34:$E$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2270,7 +2278,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-37D7-0548-889D-8F6CD5AE1EB9}"/>
+              <c16:uniqueId val="{00000002-3338-F04B-8E23-C05DF3260C71}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2357,7 +2365,94 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-37D7-0548-889D-8F6CD5AE1EB9}"/>
+              <c16:uniqueId val="{00000003-3338-F04B-8E23-C05DF3260C71}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Query Evaluation V2'!$A$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>table-sst-dc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Query Evaluation V2'!$B$31:$E$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Query Evaluation V2'!$B$36:$E$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8.8199999999999997E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3077999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4074E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5886999999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-3338-F04B-8E23-C05DF3260C71}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2369,15 +2464,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="94354191"/>
-        <c:axId val="149692879"/>
+        <c:axId val="1693629456"/>
+        <c:axId val="1694176240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="94354191"/>
+        <c:axId val="1693629456"/>
         <c:scaling>
-          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:min val="10"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2402,7 +2495,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -2416,11 +2509,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB" sz="1500"/>
-                  <a:t>No.</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="1500" baseline="0"/>
-                  <a:t> of Requests</a:t>
+                  <a:t>Number of Requests</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2438,7 +2527,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -2491,12 +2580,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="149692879"/>
+        <c:crossAx val="1694176240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="149692879"/>
+        <c:axId val="1694176240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2523,7 +2612,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -2536,10 +2625,9 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB" sz="1500" baseline="0"/>
-                  <a:t>Tail Latency (s)</a:t>
+                  <a:rPr lang="en-GB" sz="1500"/>
+                  <a:t>Tail Latency</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-GB" sz="1500"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2556,7 +2644,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -2609,7 +2697,705 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94354191"/>
+        <c:crossAx val="1693629456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1300" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Query Evaluation V2'!$A$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>stock</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Query Evaluation V2'!$B$31:$E$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Query Evaluation V2'!$B$32:$E$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7.7800000000000005E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.7900000000000005E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.1799999999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.1799999999999998E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A2B8-CB49-AA2D-9D7BDD944ED3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Query Evaluation V2'!$A$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>table-pm-dc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Query Evaluation V2'!$B$31:$E$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Query Evaluation V2'!$B$34:$E$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.9580000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.8938999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.2419999999999993E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.1221999999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A2B8-CB49-AA2D-9D7BDD944ED3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Query Evaluation V2'!$A$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>table-sst</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Query Evaluation V2'!$B$31:$E$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Query Evaluation V2'!$B$35:$E$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.8630000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.8311E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1551000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.1411000000000001E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-A2B8-CB49-AA2D-9D7BDD944ED3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Query Evaluation V2'!$A$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>table-sst-dc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Query Evaluation V2'!$B$31:$E$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Query Evaluation V2'!$B$36:$E$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8.8199999999999997E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3077999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4074E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5886999999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-A2B8-CB49-AA2D-9D7BDD944ED3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1689593824"/>
+        <c:axId val="1689595472"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1689593824"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="10"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1500"/>
+                  <a:t>NUmber of Requests</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1300" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1689595472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1689595472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1500"/>
+                  <a:t>Tail Latency</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1300" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1689593824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6965,6 +7751,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -7789,6 +8615,522 @@
 </file>
 
 <file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style11.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -12718,29 +14060,27 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>679450</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>806450</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>425450</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="11" name="Chart 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B2A5453-F931-0146-B0DA-47DA9131BE85}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D18F6D09-C91A-6747-B72B-96153E6156DE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -12756,29 +14096,27 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>273050</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="12" name="Chart 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4517DAB-4A38-B842-A40B-546286D059E0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54F6B08F-0D60-874B-9F41-33055C178247}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -12787,6 +14125,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>82550</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>527050</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="Chart 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F5BE6ED-2290-1A4A-9DED-0F0DDA721BC8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -13197,10 +14571,10 @@
       <c r="N4">
         <v>640541</v>
       </c>
-      <c r="Y4" s="28" t="s">
+      <c r="Y4" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="Z4" s="29" t="s">
+      <c r="Z4" s="33" t="s">
         <v>53</v>
       </c>
       <c r="AA4" s="10">
@@ -13272,8 +14646,8 @@
         <f>Q5*10</f>
         <v>0.23202608</v>
       </c>
-      <c r="Y5" s="28"/>
-      <c r="Z5" s="30"/>
+      <c r="Y5" s="29"/>
+      <c r="Z5" s="34"/>
       <c r="AA5" s="10">
         <v>2</v>
       </c>
@@ -13343,8 +14717,8 @@
         <f t="shared" ref="W6:W8" si="4">Q6*10</f>
         <v>44.84491688</v>
       </c>
-      <c r="Y6" s="28"/>
-      <c r="Z6" s="30"/>
+      <c r="Y6" s="29"/>
+      <c r="Z6" s="34"/>
       <c r="AA6" s="10">
         <v>3</v>
       </c>
@@ -13414,8 +14788,8 @@
         <f t="shared" si="4"/>
         <v>16.345038880000001</v>
       </c>
-      <c r="Y7" s="28"/>
-      <c r="Z7" s="30"/>
+      <c r="Y7" s="29"/>
+      <c r="Z7" s="34"/>
       <c r="AA7" s="10">
         <v>4</v>
       </c>
@@ -13487,8 +14861,8 @@
         <f t="shared" si="4"/>
         <v>0.15918689999999999</v>
       </c>
-      <c r="Y8" s="28"/>
-      <c r="Z8" s="31"/>
+      <c r="Y8" s="29"/>
+      <c r="Z8" s="35"/>
       <c r="AA8" s="10" t="s">
         <v>48</v>
       </c>
@@ -13529,8 +14903,8 @@
       <c r="H9">
         <v>2.8</v>
       </c>
-      <c r="Y9" s="28"/>
-      <c r="Z9" s="32" t="s">
+      <c r="Y9" s="29"/>
+      <c r="Z9" s="30" t="s">
         <v>54</v>
       </c>
       <c r="AA9" s="13">
@@ -13549,8 +14923,8 @@
       <c r="AG9" s="3"/>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="Y10" s="28"/>
-      <c r="Z10" s="33"/>
+      <c r="Y10" s="29"/>
+      <c r="Z10" s="31"/>
       <c r="AA10" s="13">
         <v>2</v>
       </c>
@@ -13570,8 +14944,8 @@
       <c r="C11" t="s">
         <v>9</v>
       </c>
-      <c r="Y11" s="28"/>
-      <c r="Z11" s="33"/>
+      <c r="Y11" s="29"/>
+      <c r="Z11" s="31"/>
       <c r="AA11" s="13">
         <v>3</v>
       </c>
@@ -13603,8 +14977,8 @@
       <c r="H12" t="s">
         <v>1</v>
       </c>
-      <c r="Y12" s="28"/>
-      <c r="Z12" s="33"/>
+      <c r="Y12" s="29"/>
+      <c r="Z12" s="31"/>
       <c r="AA12" s="13">
         <v>4</v>
       </c>
@@ -13641,8 +15015,8 @@
       <c r="H13">
         <v>16.75</v>
       </c>
-      <c r="Y13" s="28"/>
-      <c r="Z13" s="34"/>
+      <c r="Y13" s="29"/>
+      <c r="Z13" s="32"/>
       <c r="AA13" s="13" t="s">
         <v>48</v>
       </c>
@@ -13668,10 +15042,10 @@
       <c r="C14" t="s">
         <v>6</v>
       </c>
-      <c r="Y14" s="28" t="s">
+      <c r="Y14" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="Z14" s="29" t="s">
+      <c r="Z14" s="33" t="s">
         <v>53</v>
       </c>
       <c r="AA14" s="10">
@@ -13698,8 +15072,8 @@
       <c r="M15" t="s">
         <v>56</v>
       </c>
-      <c r="Y15" s="28"/>
-      <c r="Z15" s="30"/>
+      <c r="Y15" s="29"/>
+      <c r="Z15" s="34"/>
       <c r="AA15" s="10">
         <v>2</v>
       </c>
@@ -13721,8 +15095,8 @@
       <c r="M16" t="s">
         <v>55</v>
       </c>
-      <c r="Y16" s="28"/>
-      <c r="Z16" s="30"/>
+      <c r="Y16" s="29"/>
+      <c r="Z16" s="34"/>
       <c r="AA16" s="10">
         <v>3</v>
       </c>
@@ -13744,8 +15118,8 @@
       <c r="M17" t="s">
         <v>26</v>
       </c>
-      <c r="Y17" s="28"/>
-      <c r="Z17" s="30"/>
+      <c r="Y17" s="29"/>
+      <c r="Z17" s="34"/>
       <c r="AA17" s="10">
         <v>4</v>
       </c>
@@ -13777,8 +15151,8 @@
       <c r="Q18" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="Y18" s="28"/>
-      <c r="Z18" s="31"/>
+      <c r="Y18" s="29"/>
+      <c r="Z18" s="35"/>
       <c r="AA18" s="10" t="s">
         <v>48</v>
       </c>
@@ -13817,8 +15191,8 @@
       <c r="Q19" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="Y19" s="28"/>
-      <c r="Z19" s="32" t="s">
+      <c r="Y19" s="29"/>
+      <c r="Z19" s="30" t="s">
         <v>54</v>
       </c>
       <c r="AA19" s="13">
@@ -13855,8 +15229,8 @@
       <c r="Q20" s="3">
         <v>1</v>
       </c>
-      <c r="Y20" s="28"/>
-      <c r="Z20" s="33"/>
+      <c r="Y20" s="29"/>
+      <c r="Z20" s="31"/>
       <c r="AA20" s="13">
         <v>2</v>
       </c>
@@ -13891,8 +15265,8 @@
       <c r="Q21" s="3">
         <v>25</v>
       </c>
-      <c r="Y21" s="28"/>
-      <c r="Z21" s="33"/>
+      <c r="Y21" s="29"/>
+      <c r="Z21" s="31"/>
       <c r="AA21" s="13">
         <v>3</v>
       </c>
@@ -13927,8 +15301,8 @@
       <c r="Q22" s="3">
         <v>15</v>
       </c>
-      <c r="Y22" s="28"/>
-      <c r="Z22" s="33"/>
+      <c r="Y22" s="29"/>
+      <c r="Z22" s="31"/>
       <c r="AA22" s="13">
         <v>4</v>
       </c>
@@ -13963,8 +15337,8 @@
       <c r="Q23" s="3">
         <v>1</v>
       </c>
-      <c r="Y23" s="28"/>
-      <c r="Z23" s="34"/>
+      <c r="Y23" s="29"/>
+      <c r="Z23" s="32"/>
       <c r="AA23" s="13" t="s">
         <v>48</v>
       </c>
@@ -13993,10 +15367,10 @@
       <c r="U24" t="s">
         <v>41</v>
       </c>
-      <c r="Y24" s="28" t="s">
+      <c r="Y24" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="Z24" s="29" t="s">
+      <c r="Z24" s="33" t="s">
         <v>53</v>
       </c>
       <c r="AA24" s="10">
@@ -14023,8 +15397,8 @@
       <c r="U25" t="s">
         <v>46</v>
       </c>
-      <c r="Y25" s="28"/>
-      <c r="Z25" s="30"/>
+      <c r="Y25" s="29"/>
+      <c r="Z25" s="34"/>
       <c r="AA25" s="10">
         <v>2</v>
       </c>
@@ -14062,8 +15436,8 @@
       <c r="W26" t="s">
         <v>51</v>
       </c>
-      <c r="Y26" s="28"/>
-      <c r="Z26" s="30"/>
+      <c r="Y26" s="29"/>
+      <c r="Z26" s="34"/>
       <c r="AA26" s="10">
         <v>3</v>
       </c>
@@ -14098,8 +15472,8 @@
       <c r="U27" t="s">
         <v>43</v>
       </c>
-      <c r="Y27" s="28"/>
-      <c r="Z27" s="30"/>
+      <c r="Y27" s="29"/>
+      <c r="Z27" s="34"/>
       <c r="AA27" s="10">
         <v>4</v>
       </c>
@@ -14141,8 +15515,8 @@
       <c r="U28" t="s">
         <v>44</v>
       </c>
-      <c r="Y28" s="28"/>
-      <c r="Z28" s="31"/>
+      <c r="Y28" s="29"/>
+      <c r="Z28" s="35"/>
       <c r="AA28" s="10" t="s">
         <v>48</v>
       </c>
@@ -14184,8 +15558,8 @@
       <c r="Q29" s="3">
         <v>5</v>
       </c>
-      <c r="Y29" s="28"/>
-      <c r="Z29" s="32" t="s">
+      <c r="Y29" s="29"/>
+      <c r="Z29" s="30" t="s">
         <v>54</v>
       </c>
       <c r="AA29" s="13">
@@ -14222,8 +15596,8 @@
       <c r="Q30" s="3">
         <v>2</v>
       </c>
-      <c r="Y30" s="28"/>
-      <c r="Z30" s="33"/>
+      <c r="Y30" s="29"/>
+      <c r="Z30" s="31"/>
       <c r="AA30" s="13">
         <v>2</v>
       </c>
@@ -14258,8 +15632,8 @@
       <c r="Q31" s="3">
         <v>1</v>
       </c>
-      <c r="Y31" s="28"/>
-      <c r="Z31" s="33"/>
+      <c r="Y31" s="29"/>
+      <c r="Z31" s="31"/>
       <c r="AA31" s="13">
         <v>3</v>
       </c>
@@ -14278,8 +15652,8 @@
       <c r="AG31" s="3"/>
     </row>
     <row r="32" spans="13:33" x14ac:dyDescent="0.2">
-      <c r="Y32" s="28"/>
-      <c r="Z32" s="33"/>
+      <c r="Y32" s="29"/>
+      <c r="Z32" s="31"/>
       <c r="AA32" s="13">
         <v>4</v>
       </c>
@@ -14304,8 +15678,8 @@
       <c r="T33">
         <v>770839982</v>
       </c>
-      <c r="Y33" s="28"/>
-      <c r="Z33" s="34"/>
+      <c r="Y33" s="29"/>
+      <c r="Z33" s="32"/>
       <c r="AA33" s="13" t="s">
         <v>48</v>
       </c>
@@ -14340,10 +15714,10 @@
       <c r="T34" s="2">
         <v>26843545600</v>
       </c>
-      <c r="Y34" s="28" t="s">
+      <c r="Y34" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="Z34" s="29" t="s">
+      <c r="Z34" s="33" t="s">
         <v>53</v>
       </c>
       <c r="AA34" s="10">
@@ -14377,8 +15751,8 @@
       <c r="W35" t="s">
         <v>51</v>
       </c>
-      <c r="Y35" s="28"/>
-      <c r="Z35" s="30"/>
+      <c r="Y35" s="29"/>
+      <c r="Z35" s="34"/>
       <c r="AA35" s="10">
         <v>2</v>
       </c>
@@ -14406,8 +15780,8 @@
       <c r="T36" s="21">
         <v>21474836480</v>
       </c>
-      <c r="Y36" s="28"/>
-      <c r="Z36" s="30"/>
+      <c r="Y36" s="29"/>
+      <c r="Z36" s="34"/>
       <c r="AA36" s="10">
         <v>3</v>
       </c>
@@ -14447,8 +15821,8 @@
         <f>T34/T36</f>
         <v>1.25</v>
       </c>
-      <c r="Y37" s="28"/>
-      <c r="Z37" s="30"/>
+      <c r="Y37" s="29"/>
+      <c r="Z37" s="34"/>
       <c r="AA37" s="10">
         <v>4</v>
       </c>
@@ -14484,8 +15858,8 @@
         <f>Q38/(10^9)</f>
         <v>0.44970119600000003</v>
       </c>
-      <c r="Y38" s="28"/>
-      <c r="Z38" s="31"/>
+      <c r="Y38" s="29"/>
+      <c r="Z38" s="35"/>
       <c r="AA38" s="10" t="s">
         <v>48</v>
       </c>
@@ -14517,8 +15891,8 @@
       <c r="N39">
         <v>196.46</v>
       </c>
-      <c r="Y39" s="28"/>
-      <c r="Z39" s="32" t="s">
+      <c r="Y39" s="29"/>
+      <c r="Z39" s="30" t="s">
         <v>54</v>
       </c>
       <c r="AA39" s="13">
@@ -14550,8 +15924,8 @@
         <f>Q40/10^9</f>
         <v>4.9207099999999997E-2</v>
       </c>
-      <c r="Y40" s="28"/>
-      <c r="Z40" s="33"/>
+      <c r="Y40" s="29"/>
+      <c r="Z40" s="31"/>
       <c r="AA40" s="13">
         <v>2</v>
       </c>
@@ -14581,8 +15955,8 @@
         <f>Q41/10^9</f>
         <v>0.38889000000000001</v>
       </c>
-      <c r="Y41" s="28"/>
-      <c r="Z41" s="33"/>
+      <c r="Y41" s="29"/>
+      <c r="Z41" s="31"/>
       <c r="AA41" s="13">
         <v>3</v>
       </c>
@@ -14602,8 +15976,8 @@
     </row>
     <row r="42" spans="13:33" x14ac:dyDescent="0.2">
       <c r="R42" s="5"/>
-      <c r="Y42" s="28"/>
-      <c r="Z42" s="33"/>
+      <c r="Y42" s="29"/>
+      <c r="Z42" s="31"/>
       <c r="AA42" s="13">
         <v>4</v>
       </c>
@@ -14623,8 +15997,8 @@
     </row>
     <row r="43" spans="13:33" x14ac:dyDescent="0.2">
       <c r="R43" s="5"/>
-      <c r="Y43" s="28"/>
-      <c r="Z43" s="34"/>
+      <c r="Y43" s="29"/>
+      <c r="Z43" s="32"/>
       <c r="AA43" s="13" t="s">
         <v>48</v>
       </c>
@@ -14656,10 +16030,10 @@
       <c r="N44" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="Y44" s="28" t="s">
+      <c r="Y44" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="Z44" s="29" t="s">
+      <c r="Z44" s="33" t="s">
         <v>53</v>
       </c>
       <c r="AA44" s="10">
@@ -14679,8 +16053,8 @@
         <v>15.93</v>
       </c>
       <c r="R45" s="5"/>
-      <c r="Y45" s="28"/>
-      <c r="Z45" s="30"/>
+      <c r="Y45" s="29"/>
+      <c r="Z45" s="34"/>
       <c r="AA45" s="10">
         <v>2</v>
       </c>
@@ -14697,8 +16071,8 @@
       <c r="N46" s="3">
         <v>51.41</v>
       </c>
-      <c r="Y46" s="28"/>
-      <c r="Z46" s="30"/>
+      <c r="Y46" s="29"/>
+      <c r="Z46" s="34"/>
       <c r="AA46" s="10">
         <v>3</v>
       </c>
@@ -14715,8 +16089,8 @@
       <c r="N47" s="3">
         <v>197.34</v>
       </c>
-      <c r="Y47" s="28"/>
-      <c r="Z47" s="30"/>
+      <c r="Y47" s="29"/>
+      <c r="Z47" s="34"/>
       <c r="AA47" s="10">
         <v>4</v>
       </c>
@@ -14733,8 +16107,8 @@
       <c r="N48" s="7">
         <v>188.89</v>
       </c>
-      <c r="Y48" s="28"/>
-      <c r="Z48" s="31"/>
+      <c r="Y48" s="29"/>
+      <c r="Z48" s="35"/>
       <c r="AA48" s="10" t="s">
         <v>48</v>
       </c>
@@ -14760,8 +16134,8 @@
       </c>
     </row>
     <row r="49" spans="25:51" ht="18" x14ac:dyDescent="0.2">
-      <c r="Y49" s="28"/>
-      <c r="Z49" s="32" t="s">
+      <c r="Y49" s="29"/>
+      <c r="Z49" s="30" t="s">
         <v>54</v>
       </c>
       <c r="AA49" s="13">
@@ -14779,7 +16153,7 @@
       <c r="AE49" s="27">
         <v>11.23</v>
       </c>
-      <c r="AF49" s="35">
+      <c r="AF49" s="28">
         <v>62.33</v>
       </c>
       <c r="AG49" s="3">
@@ -14788,8 +16162,8 @@
       </c>
     </row>
     <row r="50" spans="25:51" x14ac:dyDescent="0.2">
-      <c r="Y50" s="28"/>
-      <c r="Z50" s="33"/>
+      <c r="Y50" s="29"/>
+      <c r="Z50" s="31"/>
       <c r="AA50" s="13">
         <v>2</v>
       </c>
@@ -14800,8 +16174,8 @@
       <c r="AG50" s="3"/>
     </row>
     <row r="51" spans="25:51" x14ac:dyDescent="0.2">
-      <c r="Y51" s="28"/>
-      <c r="Z51" s="33"/>
+      <c r="Y51" s="29"/>
+      <c r="Z51" s="31"/>
       <c r="AA51" s="13">
         <v>3</v>
       </c>
@@ -14812,8 +16186,8 @@
       <c r="AG51" s="3"/>
     </row>
     <row r="52" spans="25:51" x14ac:dyDescent="0.2">
-      <c r="Y52" s="28"/>
-      <c r="Z52" s="33"/>
+      <c r="Y52" s="29"/>
+      <c r="Z52" s="31"/>
       <c r="AA52" s="13">
         <v>4</v>
       </c>
@@ -14824,8 +16198,8 @@
       <c r="AG52" s="3"/>
     </row>
     <row r="53" spans="25:51" x14ac:dyDescent="0.2">
-      <c r="Y53" s="28"/>
-      <c r="Z53" s="34"/>
+      <c r="Y53" s="29"/>
+      <c r="Z53" s="32"/>
       <c r="AA53" s="13" t="s">
         <v>48</v>
       </c>
@@ -15420,12 +16794,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="Y4:Y13"/>
-    <mergeCell ref="Z9:Z13"/>
-    <mergeCell ref="Z4:Z8"/>
-    <mergeCell ref="Y14:Y23"/>
-    <mergeCell ref="Z14:Z18"/>
-    <mergeCell ref="Z19:Z23"/>
     <mergeCell ref="Y44:Y53"/>
     <mergeCell ref="Z44:Z48"/>
     <mergeCell ref="Z49:Z53"/>
@@ -15435,6 +16803,12 @@
     <mergeCell ref="Y34:Y43"/>
     <mergeCell ref="Z34:Z38"/>
     <mergeCell ref="Z39:Z43"/>
+    <mergeCell ref="Y4:Y13"/>
+    <mergeCell ref="Z9:Z13"/>
+    <mergeCell ref="Z4:Z8"/>
+    <mergeCell ref="Y14:Y23"/>
+    <mergeCell ref="Z14:Z18"/>
+    <mergeCell ref="Z19:Z23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -16645,8 +18019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F1E6D4B-CBE1-6040-B05A-6A93103A9872}">
   <dimension ref="A1:W36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="W8" sqref="W8"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="S41" sqref="S41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16768,16 +18142,16 @@
         <v>98</v>
       </c>
       <c r="T3" s="27">
-        <v>7.7590000000000003E-3</v>
+        <v>4.0260000000000001E-3</v>
       </c>
       <c r="U3" s="27">
-        <v>0.25437399999999999</v>
+        <v>0.11088199999999999</v>
       </c>
       <c r="V3" s="27">
-        <v>2.09659</v>
+        <v>1.3184199999999999</v>
       </c>
       <c r="W3" s="27">
-        <v>17.8155</v>
+        <v>15.587400000000001</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
@@ -16843,19 +18217,19 @@
       </c>
       <c r="T4">
         <f>T3/T2</f>
-        <v>7.7590000000000005E-4</v>
+        <v>4.0260000000000003E-4</v>
       </c>
       <c r="U4">
         <f>U3/U2</f>
-        <v>2.5437400000000001E-3</v>
+        <v>1.1088199999999999E-3</v>
       </c>
       <c r="V4">
         <f>V3/V2</f>
-        <v>2.0965899999999997E-3</v>
+        <v>1.3184199999999998E-3</v>
       </c>
       <c r="W4">
-        <f t="shared" ref="V4:W4" si="3">W3/W2</f>
-        <v>1.78155E-3</v>
+        <f t="shared" ref="W4" si="3">W3/W2</f>
+        <v>1.5587400000000001E-3</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
@@ -16921,19 +18295,19 @@
       </c>
       <c r="T5">
         <f>1/T4</f>
-        <v>1288.8258796236628</v>
+        <v>2483.8549428713363</v>
       </c>
       <c r="U5">
         <f t="shared" ref="U5:W5" si="7">1/U4</f>
-        <v>393.12193856290344</v>
+        <v>901.85963456647607</v>
       </c>
       <c r="V5">
         <f>1/V4</f>
-        <v>476.96497646177846</v>
+        <v>758.48363950789587</v>
       </c>
       <c r="W5">
         <f t="shared" si="7"/>
-        <v>561.30897252392583</v>
+        <v>641.543811026855</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="18" x14ac:dyDescent="0.2">
@@ -16968,10 +18342,10 @@
         <v>101</v>
       </c>
       <c r="T6" s="27">
-        <v>2.0799999999999999E-4</v>
+        <v>2.0599999999999999E-4</v>
       </c>
       <c r="U6" s="27">
-        <v>9.0000000000000006E-5</v>
+        <v>5.0000000000000002E-5</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="18" x14ac:dyDescent="0.2">
@@ -17024,16 +18398,16 @@
         <v>102</v>
       </c>
       <c r="T7" s="27">
-        <v>2.885E-3</v>
+        <v>8.8199999999999997E-4</v>
       </c>
       <c r="U7" s="27">
-        <v>5.1577999999999999E-2</v>
+        <v>1.3077999999999999E-2</v>
       </c>
       <c r="V7" s="27">
-        <v>0.27768100000000001</v>
+        <v>6.2973000000000001E-2</v>
       </c>
       <c r="W7" s="27">
-        <v>0.50517599999999996</v>
+        <v>0.41688399999999998</v>
       </c>
     </row>
     <row r="8" spans="1:23" ht="18" x14ac:dyDescent="0.2">
@@ -17086,16 +18460,16 @@
         <v>103</v>
       </c>
       <c r="T8" s="27">
-        <v>2.885E-3</v>
+        <v>8.8199999999999997E-4</v>
       </c>
       <c r="U8" s="27">
-        <v>5.1577999999999999E-2</v>
+        <v>1.3077999999999999E-2</v>
       </c>
       <c r="V8" s="27">
-        <v>2.0629000000000002E-2</v>
+        <v>1.4074E-2</v>
       </c>
       <c r="W8" s="27">
-        <v>1.7876E-2</v>
+        <v>1.5886999999999998E-2</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
@@ -17382,19 +18756,19 @@
       </c>
       <c r="B28">
         <f>T5</f>
-        <v>1288.8258796236628</v>
+        <v>2483.8549428713363</v>
       </c>
       <c r="C28">
         <f t="shared" ref="C28:E28" si="12">U5</f>
-        <v>393.12193856290344</v>
+        <v>901.85963456647607</v>
       </c>
       <c r="D28">
         <f t="shared" si="12"/>
-        <v>476.96497646177846</v>
+        <v>758.48363950789587</v>
       </c>
       <c r="E28">
         <f t="shared" si="12"/>
-        <v>561.30897252392583</v>
+        <v>641.543811026855</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -17509,19 +18883,19 @@
       </c>
       <c r="B36">
         <f>T8</f>
-        <v>2.885E-3</v>
+        <v>8.8199999999999997E-4</v>
       </c>
       <c r="C36">
         <f t="shared" ref="C36:D36" si="13">U8</f>
-        <v>5.1577999999999999E-2</v>
+        <v>1.3077999999999999E-2</v>
       </c>
       <c r="D36">
         <f t="shared" si="13"/>
-        <v>2.0629000000000002E-2</v>
+        <v>1.4074E-2</v>
       </c>
       <c r="E36">
         <f>W8</f>
-        <v>1.7876E-2</v>
+        <v>1.5886999999999998E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>